<commit_message>
Updated to include all 2024-25 games and Utah NHL
</commit_message>
<xml_diff>
--- a/team_venue_info.xlsx
+++ b/team_venue_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hunte\Documents\Projects\api-sports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300E56C5-F914-463F-AE62-D308AF05007D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02075905-F722-4EDC-A070-D4B9EB0BE8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4DE514D5-098E-4250-809A-53ED6767566D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4DE514D5-098E-4250-809A-53ED6767566D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="625">
   <si>
     <t>MLB</t>
   </si>
@@ -1265,9 +1265,6 @@
     <t>Anaheim</t>
   </si>
   <si>
-    <t>Arizona Coyotes</t>
-  </si>
-  <si>
     <t>Boston Bruins</t>
   </si>
   <si>
@@ -1751,12 +1748,6 @@
     <t>2695 E Katella Ave, Anaheim, CA 92806</t>
   </si>
   <si>
-    <t>Desert Diamond Arena</t>
-  </si>
-  <si>
-    <t>9400 W Maryland Ave, Glendale, AZ 85305</t>
-  </si>
-  <si>
     <t>1 Seymour H Knox III Plaza, Buffalo, NY 14203</t>
   </si>
   <si>
@@ -1914,6 +1905,12 @@
   </si>
   <si>
     <t>Seattle Kraken</t>
+  </si>
+  <si>
+    <t>Delta Center</t>
+  </si>
+  <si>
+    <t>301 S Temple, Salt Lake City, UT 84101</t>
   </si>
 </sst>
 </file>
@@ -2294,8 +2291,8 @@
   <dimension ref="A1:H155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B149" sqref="B149"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2312,28 +2309,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>612</v>
+      </c>
+      <c r="B1" t="s">
+        <v>613</v>
+      </c>
+      <c r="C1" t="s">
+        <v>614</v>
+      </c>
+      <c r="D1" t="s">
         <v>615</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>616</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>617</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>618</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>619</v>
-      </c>
-      <c r="F1" t="s">
-        <v>620</v>
-      </c>
-      <c r="G1" t="s">
-        <v>621</v>
-      </c>
-      <c r="H1" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2359,7 +2356,7 @@
         <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2385,7 +2382,7 @@
         <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2411,7 +2408,7 @@
         <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2437,7 +2434,7 @@
         <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2463,7 +2460,7 @@
         <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2489,7 +2486,7 @@
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2515,7 +2512,7 @@
         <v>6</v>
       </c>
       <c r="H8" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2541,7 +2538,7 @@
         <v>6</v>
       </c>
       <c r="H9" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2567,7 +2564,7 @@
         <v>6</v>
       </c>
       <c r="H10" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2593,7 +2590,7 @@
         <v>6</v>
       </c>
       <c r="H11" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2619,7 +2616,7 @@
         <v>6</v>
       </c>
       <c r="H12" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2645,7 +2642,7 @@
         <v>6</v>
       </c>
       <c r="H13" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2671,7 +2668,7 @@
         <v>6</v>
       </c>
       <c r="H14" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2697,7 +2694,7 @@
         <v>6</v>
       </c>
       <c r="H15" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2723,7 +2720,7 @@
         <v>6</v>
       </c>
       <c r="H16" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2749,7 +2746,7 @@
         <v>6</v>
       </c>
       <c r="H17" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2775,7 +2772,7 @@
         <v>6</v>
       </c>
       <c r="H18" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2801,7 +2798,7 @@
         <v>6</v>
       </c>
       <c r="H19" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2827,7 +2824,7 @@
         <v>6</v>
       </c>
       <c r="H20" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2853,7 +2850,7 @@
         <v>6</v>
       </c>
       <c r="H21" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2879,7 +2876,7 @@
         <v>6</v>
       </c>
       <c r="H22" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2905,7 +2902,7 @@
         <v>6</v>
       </c>
       <c r="H23" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2931,7 +2928,7 @@
         <v>6</v>
       </c>
       <c r="H24" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2957,7 +2954,7 @@
         <v>6</v>
       </c>
       <c r="H25" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2983,7 +2980,7 @@
         <v>6</v>
       </c>
       <c r="H26" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -3009,7 +3006,7 @@
         <v>6</v>
       </c>
       <c r="H27" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -3035,7 +3032,7 @@
         <v>6</v>
       </c>
       <c r="H28" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -3061,7 +3058,7 @@
         <v>6</v>
       </c>
       <c r="H29" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -3087,7 +3084,7 @@
         <v>132</v>
       </c>
       <c r="H30" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -3113,7 +3110,7 @@
         <v>6</v>
       </c>
       <c r="H31" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -3139,7 +3136,7 @@
         <v>6</v>
       </c>
       <c r="H32" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -3165,7 +3162,7 @@
         <v>6</v>
       </c>
       <c r="H33" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -3173,7 +3170,7 @@
         <v>137</v>
       </c>
       <c r="B34" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="C34" t="s">
         <v>146</v>
@@ -3191,7 +3188,7 @@
         <v>132</v>
       </c>
       <c r="H34" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3217,7 +3214,7 @@
         <v>6</v>
       </c>
       <c r="H35" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -3243,7 +3240,7 @@
         <v>6</v>
       </c>
       <c r="H36" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -3269,7 +3266,7 @@
         <v>6</v>
       </c>
       <c r="H37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -3295,7 +3292,7 @@
         <v>6</v>
       </c>
       <c r="H38" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3321,7 +3318,7 @@
         <v>6</v>
       </c>
       <c r="H39" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -3347,7 +3344,7 @@
         <v>6</v>
       </c>
       <c r="H40" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -3373,7 +3370,7 @@
         <v>6</v>
       </c>
       <c r="H41" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -3399,7 +3396,7 @@
         <v>6</v>
       </c>
       <c r="H42" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -3425,7 +3422,7 @@
         <v>6</v>
       </c>
       <c r="H43" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -3451,7 +3448,7 @@
         <v>6</v>
       </c>
       <c r="H44" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3477,7 +3474,7 @@
         <v>6</v>
       </c>
       <c r="H45" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -3503,7 +3500,7 @@
         <v>6</v>
       </c>
       <c r="H46" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3529,7 +3526,7 @@
         <v>6</v>
       </c>
       <c r="H47" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3555,7 +3552,7 @@
         <v>6</v>
       </c>
       <c r="H48" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -3581,7 +3578,7 @@
         <v>6</v>
       </c>
       <c r="H49" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -3607,7 +3604,7 @@
         <v>6</v>
       </c>
       <c r="H50" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -3633,7 +3630,7 @@
         <v>6</v>
       </c>
       <c r="H51" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -3659,7 +3656,7 @@
         <v>6</v>
       </c>
       <c r="H52" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -3685,7 +3682,7 @@
         <v>6</v>
       </c>
       <c r="H53" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -3711,7 +3708,7 @@
         <v>6</v>
       </c>
       <c r="H54" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -3737,7 +3734,7 @@
         <v>6</v>
       </c>
       <c r="H55" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -3763,7 +3760,7 @@
         <v>6</v>
       </c>
       <c r="H56" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -3789,7 +3786,7 @@
         <v>6</v>
       </c>
       <c r="H57" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -3815,7 +3812,7 @@
         <v>6</v>
       </c>
       <c r="H58" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -3841,7 +3838,7 @@
         <v>132</v>
       </c>
       <c r="H59" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -3867,7 +3864,7 @@
         <v>132</v>
       </c>
       <c r="H60" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -3893,7 +3890,7 @@
         <v>6</v>
       </c>
       <c r="H61" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -3919,7 +3916,7 @@
         <v>6</v>
       </c>
       <c r="H62" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -3945,7 +3942,7 @@
         <v>6</v>
       </c>
       <c r="H63" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -3971,7 +3968,7 @@
         <v>6</v>
       </c>
       <c r="H64" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -3997,7 +3994,7 @@
         <v>6</v>
       </c>
       <c r="H65" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -4023,7 +4020,7 @@
         <v>6</v>
       </c>
       <c r="H66" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -4049,7 +4046,7 @@
         <v>6</v>
       </c>
       <c r="H67" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -4075,7 +4072,7 @@
         <v>6</v>
       </c>
       <c r="H68" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -4101,7 +4098,7 @@
         <v>6</v>
       </c>
       <c r="H69" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -4127,7 +4124,7 @@
         <v>6</v>
       </c>
       <c r="H70" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -4153,7 +4150,7 @@
         <v>6</v>
       </c>
       <c r="H71" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -4179,7 +4176,7 @@
         <v>6</v>
       </c>
       <c r="H72" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -4205,7 +4202,7 @@
         <v>6</v>
       </c>
       <c r="H73" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -4231,7 +4228,7 @@
         <v>6</v>
       </c>
       <c r="H74" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -4257,7 +4254,7 @@
         <v>6</v>
       </c>
       <c r="H75" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -4283,7 +4280,7 @@
         <v>6</v>
       </c>
       <c r="H76" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -4309,7 +4306,7 @@
         <v>6</v>
       </c>
       <c r="H77" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -4335,7 +4332,7 @@
         <v>6</v>
       </c>
       <c r="H78" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -4361,7 +4358,7 @@
         <v>6</v>
       </c>
       <c r="H79" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -4387,7 +4384,7 @@
         <v>6</v>
       </c>
       <c r="H80" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -4413,7 +4410,7 @@
         <v>6</v>
       </c>
       <c r="H81" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -4439,7 +4436,7 @@
         <v>6</v>
       </c>
       <c r="H82" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -4465,7 +4462,7 @@
         <v>6</v>
       </c>
       <c r="H83" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -4491,7 +4488,7 @@
         <v>6</v>
       </c>
       <c r="H84" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -4517,7 +4514,7 @@
         <v>6</v>
       </c>
       <c r="H85" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -4543,7 +4540,7 @@
         <v>6</v>
       </c>
       <c r="H86" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -4569,7 +4566,7 @@
         <v>6</v>
       </c>
       <c r="H87" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -4595,7 +4592,7 @@
         <v>132</v>
       </c>
       <c r="H88" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -4621,7 +4618,7 @@
         <v>6</v>
       </c>
       <c r="H89" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -4647,7 +4644,7 @@
         <v>6</v>
       </c>
       <c r="H90" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -4673,7 +4670,7 @@
         <v>6</v>
       </c>
       <c r="H91" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -4699,7 +4696,7 @@
         <v>6</v>
       </c>
       <c r="H92" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -4725,7 +4722,7 @@
         <v>6</v>
       </c>
       <c r="H93" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -4751,7 +4748,7 @@
         <v>6</v>
       </c>
       <c r="H94" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -4777,7 +4774,7 @@
         <v>6</v>
       </c>
       <c r="H95" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -4803,7 +4800,7 @@
         <v>6</v>
       </c>
       <c r="H96" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -4829,7 +4826,7 @@
         <v>6</v>
       </c>
       <c r="H97" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -4855,7 +4852,7 @@
         <v>6</v>
       </c>
       <c r="H98" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -4881,7 +4878,7 @@
         <v>6</v>
       </c>
       <c r="H99" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -4907,7 +4904,7 @@
         <v>6</v>
       </c>
       <c r="H100" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -4933,7 +4930,7 @@
         <v>6</v>
       </c>
       <c r="H101" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -4959,7 +4956,7 @@
         <v>6</v>
       </c>
       <c r="H102" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -4985,7 +4982,7 @@
         <v>6</v>
       </c>
       <c r="H103" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -5011,7 +5008,7 @@
         <v>6</v>
       </c>
       <c r="H104" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -5022,7 +5019,7 @@
         <v>356</v>
       </c>
       <c r="C105" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D105" t="s">
         <v>357</v>
@@ -5037,7 +5034,7 @@
         <v>6</v>
       </c>
       <c r="H105" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -5063,7 +5060,7 @@
         <v>6</v>
       </c>
       <c r="H106" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -5089,7 +5086,7 @@
         <v>6</v>
       </c>
       <c r="H107" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -5115,7 +5112,7 @@
         <v>6</v>
       </c>
       <c r="H108" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -5141,7 +5138,7 @@
         <v>6</v>
       </c>
       <c r="H109" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -5167,7 +5164,7 @@
         <v>6</v>
       </c>
       <c r="H110" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -5193,7 +5190,7 @@
         <v>6</v>
       </c>
       <c r="H111" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -5219,7 +5216,7 @@
         <v>6</v>
       </c>
       <c r="H112" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -5245,7 +5242,7 @@
         <v>6</v>
       </c>
       <c r="H113" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -5271,7 +5268,7 @@
         <v>6</v>
       </c>
       <c r="H114" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -5297,7 +5294,7 @@
         <v>6</v>
       </c>
       <c r="H115" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -5323,7 +5320,7 @@
         <v>6</v>
       </c>
       <c r="H116" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -5349,7 +5346,7 @@
         <v>6</v>
       </c>
       <c r="H117" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -5375,7 +5372,7 @@
         <v>6</v>
       </c>
       <c r="H118" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -5401,7 +5398,7 @@
         <v>6</v>
       </c>
       <c r="H119" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -5427,7 +5424,7 @@
         <v>6</v>
       </c>
       <c r="H120" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -5453,7 +5450,7 @@
         <v>6</v>
       </c>
       <c r="H121" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -5479,7 +5476,7 @@
         <v>6</v>
       </c>
       <c r="H122" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -5505,7 +5502,7 @@
         <v>6</v>
       </c>
       <c r="H123" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -5513,25 +5510,25 @@
         <v>404</v>
       </c>
       <c r="B124" t="s">
-        <v>409</v>
+        <v>221</v>
       </c>
       <c r="C124" t="s">
-        <v>571</v>
+        <v>623</v>
       </c>
       <c r="D124" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="E124" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="F124" t="s">
-        <v>5</v>
+        <v>221</v>
       </c>
       <c r="G124" t="s">
         <v>6</v>
       </c>
       <c r="H124" t="s">
-        <v>572</v>
+        <v>624</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -5539,7 +5536,7 @@
         <v>404</v>
       </c>
       <c r="B125" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C125" t="s">
         <v>245</v>
@@ -5557,7 +5554,7 @@
         <v>6</v>
       </c>
       <c r="H125" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -5565,16 +5562,16 @@
         <v>404</v>
       </c>
       <c r="B126" t="s">
+        <v>410</v>
+      </c>
+      <c r="C126" t="s">
         <v>411</v>
       </c>
-      <c r="C126" t="s">
+      <c r="D126" t="s">
         <v>412</v>
       </c>
-      <c r="D126" t="s">
+      <c r="E126" t="s">
         <v>413</v>
-      </c>
-      <c r="E126" t="s">
-        <v>414</v>
       </c>
       <c r="F126" t="s">
         <v>84</v>
@@ -5583,7 +5580,7 @@
         <v>6</v>
       </c>
       <c r="H126" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -5591,25 +5588,25 @@
         <v>404</v>
       </c>
       <c r="B127" t="s">
+        <v>414</v>
+      </c>
+      <c r="C127" t="s">
         <v>415</v>
       </c>
-      <c r="C127" t="s">
+      <c r="D127" t="s">
         <v>416</v>
       </c>
-      <c r="D127" t="s">
+      <c r="E127" t="s">
         <v>417</v>
       </c>
-      <c r="E127" t="s">
+      <c r="F127" t="s">
         <v>418</v>
-      </c>
-      <c r="F127" t="s">
-        <v>419</v>
       </c>
       <c r="G127" t="s">
         <v>132</v>
       </c>
       <c r="H127" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -5617,16 +5614,16 @@
         <v>404</v>
       </c>
       <c r="B128" t="s">
+        <v>419</v>
+      </c>
+      <c r="C128" t="s">
         <v>420</v>
       </c>
-      <c r="C128" t="s">
+      <c r="D128" t="s">
         <v>421</v>
       </c>
-      <c r="D128" t="s">
+      <c r="E128" t="s">
         <v>422</v>
-      </c>
-      <c r="E128" t="s">
-        <v>423</v>
       </c>
       <c r="F128" t="s">
         <v>154</v>
@@ -5635,7 +5632,7 @@
         <v>6</v>
       </c>
       <c r="H128" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -5643,7 +5640,7 @@
         <v>404</v>
       </c>
       <c r="B129" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C129" t="s">
         <v>253</v>
@@ -5661,7 +5658,7 @@
         <v>6</v>
       </c>
       <c r="H129" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -5669,7 +5666,7 @@
         <v>404</v>
       </c>
       <c r="B130" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C130" t="s">
         <v>261</v>
@@ -5687,7 +5684,7 @@
         <v>6</v>
       </c>
       <c r="H130" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -5695,10 +5692,10 @@
         <v>404</v>
       </c>
       <c r="B131" t="s">
+        <v>425</v>
+      </c>
+      <c r="C131" t="s">
         <v>426</v>
-      </c>
-      <c r="C131" t="s">
-        <v>427</v>
       </c>
       <c r="D131" t="s">
         <v>163</v>
@@ -5713,7 +5710,7 @@
         <v>6</v>
       </c>
       <c r="H131" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -5721,7 +5718,7 @@
         <v>404</v>
       </c>
       <c r="B132" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C132" t="s">
         <v>257</v>
@@ -5739,7 +5736,7 @@
         <v>6</v>
       </c>
       <c r="H132" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -5747,7 +5744,7 @@
         <v>404</v>
       </c>
       <c r="B133" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C133" t="s">
         <v>263</v>
@@ -5765,7 +5762,7 @@
         <v>6</v>
       </c>
       <c r="H133" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
@@ -5773,25 +5770,25 @@
         <v>404</v>
       </c>
       <c r="B134" t="s">
+        <v>429</v>
+      </c>
+      <c r="C134" t="s">
         <v>430</v>
       </c>
-      <c r="C134" t="s">
+      <c r="D134" t="s">
         <v>431</v>
       </c>
-      <c r="D134" t="s">
+      <c r="E134" t="s">
         <v>432</v>
       </c>
-      <c r="E134" t="s">
-        <v>433</v>
-      </c>
       <c r="F134" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G134" t="s">
         <v>132</v>
       </c>
       <c r="H134" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -5799,16 +5796,16 @@
         <v>404</v>
       </c>
       <c r="B135" t="s">
+        <v>433</v>
+      </c>
+      <c r="C135" t="s">
         <v>434</v>
       </c>
-      <c r="C135" t="s">
+      <c r="D135" t="s">
         <v>435</v>
       </c>
-      <c r="D135" t="s">
+      <c r="E135" t="s">
         <v>436</v>
-      </c>
-      <c r="E135" t="s">
-        <v>437</v>
       </c>
       <c r="F135" t="s">
         <v>69</v>
@@ -5817,7 +5814,7 @@
         <v>6</v>
       </c>
       <c r="H135" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -5825,10 +5822,10 @@
         <v>404</v>
       </c>
       <c r="B136" t="s">
+        <v>437</v>
+      </c>
+      <c r="C136" t="s">
         <v>438</v>
-      </c>
-      <c r="C136" t="s">
-        <v>439</v>
       </c>
       <c r="D136" t="s">
         <v>60</v>
@@ -5843,7 +5840,7 @@
         <v>6</v>
       </c>
       <c r="H136" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -5851,10 +5848,10 @@
         <v>404</v>
       </c>
       <c r="B137" t="s">
+        <v>439</v>
+      </c>
+      <c r="C137" t="s">
         <v>440</v>
-      </c>
-      <c r="C137" t="s">
-        <v>441</v>
       </c>
       <c r="D137" t="s">
         <v>187</v>
@@ -5869,7 +5866,7 @@
         <v>6</v>
       </c>
       <c r="H137" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
@@ -5877,10 +5874,10 @@
         <v>404</v>
       </c>
       <c r="B138" t="s">
+        <v>441</v>
+      </c>
+      <c r="C138" t="s">
         <v>442</v>
-      </c>
-      <c r="C138" t="s">
-        <v>443</v>
       </c>
       <c r="D138" t="s">
         <v>147</v>
@@ -5895,7 +5892,7 @@
         <v>132</v>
       </c>
       <c r="H138" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -5903,10 +5900,10 @@
         <v>404</v>
       </c>
       <c r="B139" t="s">
+        <v>443</v>
+      </c>
+      <c r="C139" t="s">
         <v>444</v>
-      </c>
-      <c r="C139" t="s">
-        <v>445</v>
       </c>
       <c r="D139" t="s">
         <v>191</v>
@@ -5921,7 +5918,7 @@
         <v>6</v>
       </c>
       <c r="H139" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
@@ -5929,16 +5926,16 @@
         <v>404</v>
       </c>
       <c r="B140" t="s">
+        <v>445</v>
+      </c>
+      <c r="C140" t="s">
         <v>446</v>
       </c>
-      <c r="C140" t="s">
+      <c r="D140" t="s">
         <v>447</v>
       </c>
-      <c r="D140" t="s">
+      <c r="E140" t="s">
         <v>448</v>
-      </c>
-      <c r="E140" t="s">
-        <v>449</v>
       </c>
       <c r="F140" t="s">
         <v>203</v>
@@ -5947,7 +5944,7 @@
         <v>6</v>
       </c>
       <c r="H140" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
@@ -5955,7 +5952,7 @@
         <v>404</v>
       </c>
       <c r="B141" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C141" t="s">
         <v>247</v>
@@ -5973,7 +5970,7 @@
         <v>6</v>
       </c>
       <c r="H141" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
@@ -5981,16 +5978,16 @@
         <v>404</v>
       </c>
       <c r="B142" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C142" t="s">
+        <v>535</v>
+      </c>
+      <c r="D142" t="s">
         <v>536</v>
       </c>
-      <c r="D142" t="s">
+      <c r="E142" t="s">
         <v>537</v>
-      </c>
-      <c r="E142" t="s">
-        <v>538</v>
       </c>
       <c r="F142" t="s">
         <v>84</v>
@@ -5999,7 +5996,7 @@
         <v>6</v>
       </c>
       <c r="H142" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
@@ -6007,7 +6004,7 @@
         <v>404</v>
       </c>
       <c r="B143" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C143" t="s">
         <v>292</v>
@@ -6025,7 +6022,7 @@
         <v>6</v>
       </c>
       <c r="H143" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
@@ -6033,16 +6030,16 @@
         <v>404</v>
       </c>
       <c r="B144" t="s">
+        <v>451</v>
+      </c>
+      <c r="C144" t="s">
         <v>452</v>
       </c>
-      <c r="C144" t="s">
+      <c r="D144" t="s">
         <v>453</v>
       </c>
-      <c r="D144" t="s">
+      <c r="E144" t="s">
         <v>454</v>
-      </c>
-      <c r="E144" t="s">
-        <v>455</v>
       </c>
       <c r="F144" t="s">
         <v>131</v>
@@ -6051,7 +6048,7 @@
         <v>132</v>
       </c>
       <c r="H144" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -6059,7 +6056,7 @@
         <v>404</v>
       </c>
       <c r="B145" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C145" t="s">
         <v>303</v>
@@ -6077,7 +6074,7 @@
         <v>6</v>
       </c>
       <c r="H145" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
@@ -6085,10 +6082,10 @@
         <v>404</v>
       </c>
       <c r="B146" t="s">
+        <v>456</v>
+      </c>
+      <c r="C146" t="s">
         <v>457</v>
-      </c>
-      <c r="C146" t="s">
-        <v>458</v>
       </c>
       <c r="D146" t="s">
         <v>100</v>
@@ -6103,7 +6100,7 @@
         <v>6</v>
       </c>
       <c r="H146" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
@@ -6111,10 +6108,10 @@
         <v>404</v>
       </c>
       <c r="B147" t="s">
+        <v>458</v>
+      </c>
+      <c r="C147" t="s">
         <v>459</v>
-      </c>
-      <c r="C147" t="s">
-        <v>460</v>
       </c>
       <c r="D147" t="s">
         <v>224</v>
@@ -6129,7 +6126,7 @@
         <v>6</v>
       </c>
       <c r="H147" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
@@ -6137,10 +6134,10 @@
         <v>404</v>
       </c>
       <c r="B148" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="C148" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D148" t="s">
         <v>112</v>
@@ -6155,7 +6152,7 @@
         <v>6</v>
       </c>
       <c r="H148" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
@@ -6163,10 +6160,10 @@
         <v>404</v>
       </c>
       <c r="B149" t="s">
+        <v>461</v>
+      </c>
+      <c r="C149" t="s">
         <v>462</v>
-      </c>
-      <c r="C149" t="s">
-        <v>463</v>
       </c>
       <c r="D149" t="s">
         <v>117</v>
@@ -6181,7 +6178,7 @@
         <v>6</v>
       </c>
       <c r="H149" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -6189,10 +6186,10 @@
         <v>404</v>
       </c>
       <c r="B150" t="s">
+        <v>463</v>
+      </c>
+      <c r="C150" t="s">
         <v>464</v>
-      </c>
-      <c r="C150" t="s">
-        <v>465</v>
       </c>
       <c r="D150" t="s">
         <v>396</v>
@@ -6207,7 +6204,7 @@
         <v>6</v>
       </c>
       <c r="H150" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -6215,7 +6212,7 @@
         <v>404</v>
       </c>
       <c r="B151" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C151" t="s">
         <v>317</v>
@@ -6233,7 +6230,7 @@
         <v>132</v>
       </c>
       <c r="H151" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
@@ -6241,10 +6238,10 @@
         <v>404</v>
       </c>
       <c r="B152" t="s">
+        <v>466</v>
+      </c>
+      <c r="C152" t="s">
         <v>467</v>
-      </c>
-      <c r="C152" t="s">
-        <v>468</v>
       </c>
       <c r="D152" t="s">
         <v>238</v>
@@ -6259,7 +6256,7 @@
         <v>132</v>
       </c>
       <c r="H152" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -6267,10 +6264,10 @@
         <v>404</v>
       </c>
       <c r="B153" t="s">
+        <v>468</v>
+      </c>
+      <c r="C153" t="s">
         <v>469</v>
-      </c>
-      <c r="C153" t="s">
-        <v>470</v>
       </c>
       <c r="D153" t="s">
         <v>363</v>
@@ -6285,7 +6282,7 @@
         <v>6</v>
       </c>
       <c r="H153" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -6293,7 +6290,7 @@
         <v>404</v>
       </c>
       <c r="B154" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C154" t="s">
         <v>323</v>
@@ -6311,7 +6308,7 @@
         <v>6</v>
       </c>
       <c r="H154" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
@@ -6319,25 +6316,25 @@
         <v>404</v>
       </c>
       <c r="B155" t="s">
+        <v>471</v>
+      </c>
+      <c r="C155" t="s">
         <v>472</v>
       </c>
-      <c r="C155" t="s">
+      <c r="D155" t="s">
         <v>473</v>
       </c>
-      <c r="D155" t="s">
+      <c r="E155" t="s">
         <v>474</v>
       </c>
-      <c r="E155" t="s">
+      <c r="F155" t="s">
         <v>475</v>
-      </c>
-      <c r="F155" t="s">
-        <v>476</v>
       </c>
       <c r="G155" t="s">
         <v>132</v>
       </c>
       <c r="H155" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Metro areas, Tableau dashboard
Added metro areas to team venue info, views, and game finder. Started work on a Tableau dashboard.
</commit_message>
<xml_diff>
--- a/team_venue_info.xlsx
+++ b/team_venue_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hunte\Documents\Projects\api-sports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02075905-F722-4EDC-A070-D4B9EB0BE8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8B96E1-F2E4-4C8D-A33A-368CDC3EEE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4DE514D5-098E-4250-809A-53ED6767566D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="13740" windowHeight="23520" xr2:uid="{4DE514D5-098E-4250-809A-53ED6767566D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="627">
   <si>
     <t>MLB</t>
   </si>
@@ -1911,6 +1911,12 @@
   </si>
   <si>
     <t>301 S Temple, Salt Lake City, UT 84101</t>
+  </si>
+  <si>
+    <t>metro_area</t>
+  </si>
+  <si>
+    <t>Las Vegas, Nevada</t>
   </si>
 </sst>
 </file>
@@ -2288,9 +2294,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D51AA39B-ABAB-4093-BF73-448F367B6941}">
-  <dimension ref="A1:H155"/>
+  <dimension ref="A1:I155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -2303,11 +2309,12 @@
     <col min="4" max="4" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>612</v>
       </c>
@@ -2327,13 +2334,16 @@
         <v>617</v>
       </c>
       <c r="G1" t="s">
+        <v>625</v>
+      </c>
+      <c r="H1" t="s">
         <v>618</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2352,14 +2362,18 @@
       <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
-        <v>6</v>
+      <c r="G2" t="str">
+        <f>D2</f>
+        <v>Phoenix, Arizona</v>
       </c>
       <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2379,13 +2393,16 @@
         <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2404,14 +2421,18 @@
       <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="G4" t="s">
-        <v>6</v>
+      <c r="G4" t="str">
+        <f t="shared" ref="G4:G67" si="0">D4</f>
+        <v>Baltimore, Maryland</v>
       </c>
       <c r="H4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2430,14 +2451,18 @@
       <c r="F5" t="s">
         <v>21</v>
       </c>
-      <c r="G5" t="s">
-        <v>6</v>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>Boston, Massachusetts</v>
       </c>
       <c r="H5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -2456,14 +2481,18 @@
       <c r="F6" t="s">
         <v>26</v>
       </c>
-      <c r="G6" t="s">
-        <v>6</v>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>Chicago, Illinois</v>
       </c>
       <c r="H6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -2482,14 +2511,18 @@
       <c r="F7" t="s">
         <v>26</v>
       </c>
-      <c r="G7" t="s">
-        <v>6</v>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>Chicago, Illinois</v>
       </c>
       <c r="H7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -2508,14 +2541,18 @@
       <c r="F8" t="s">
         <v>33</v>
       </c>
-      <c r="G8" t="s">
-        <v>6</v>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>Cincinnati, Ohio</v>
       </c>
       <c r="H8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -2534,14 +2571,18 @@
       <c r="F9" t="s">
         <v>33</v>
       </c>
-      <c r="G9" t="s">
-        <v>6</v>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>Cleveland, Ohio</v>
       </c>
       <c r="H9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -2560,14 +2601,18 @@
       <c r="F10" t="s">
         <v>42</v>
       </c>
-      <c r="G10" t="s">
-        <v>6</v>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>Denver, Colorado</v>
       </c>
       <c r="H10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -2586,14 +2631,18 @@
       <c r="F11" t="s">
         <v>47</v>
       </c>
-      <c r="G11" t="s">
-        <v>6</v>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>Detroit, Michigan</v>
       </c>
       <c r="H11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -2612,14 +2661,18 @@
       <c r="F12" t="s">
         <v>52</v>
       </c>
-      <c r="G12" t="s">
-        <v>6</v>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>Houston, Texas</v>
       </c>
       <c r="H12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -2638,14 +2691,18 @@
       <c r="F13" t="s">
         <v>57</v>
       </c>
-      <c r="G13" t="s">
-        <v>6</v>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>Kansas City, Missouri</v>
       </c>
       <c r="H13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -2664,14 +2721,18 @@
       <c r="F14" t="s">
         <v>62</v>
       </c>
-      <c r="G14" t="s">
-        <v>6</v>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>Los Angeles, California</v>
       </c>
       <c r="H14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -2690,14 +2751,18 @@
       <c r="F15" t="s">
         <v>62</v>
       </c>
-      <c r="G15" t="s">
-        <v>6</v>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>Los Angeles, California</v>
       </c>
       <c r="H15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -2716,14 +2781,18 @@
       <c r="F16" t="s">
         <v>69</v>
       </c>
-      <c r="G16" t="s">
-        <v>6</v>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>Miami, Florida</v>
       </c>
       <c r="H16" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -2742,14 +2811,18 @@
       <c r="F17" t="s">
         <v>74</v>
       </c>
-      <c r="G17" t="s">
-        <v>6</v>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>Milwaukee, Wisconsin</v>
       </c>
       <c r="H17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -2768,14 +2841,18 @@
       <c r="F18" t="s">
         <v>79</v>
       </c>
-      <c r="G18" t="s">
-        <v>6</v>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>Minneapolis, Minnesota</v>
       </c>
       <c r="H18" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -2795,13 +2872,16 @@
         <v>84</v>
       </c>
       <c r="G19" t="s">
-        <v>6</v>
+        <v>293</v>
       </c>
       <c r="H19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -2821,13 +2901,16 @@
         <v>84</v>
       </c>
       <c r="G20" t="s">
-        <v>6</v>
+        <v>293</v>
       </c>
       <c r="H20" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -2847,13 +2930,16 @@
         <v>62</v>
       </c>
       <c r="G21" t="s">
-        <v>6</v>
+        <v>108</v>
       </c>
       <c r="H21" t="s">
+        <v>6</v>
+      </c>
+      <c r="I21" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -2872,14 +2958,18 @@
       <c r="F22" t="s">
         <v>97</v>
       </c>
-      <c r="G22" t="s">
-        <v>6</v>
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>Philadelphia, Pennsylvania</v>
       </c>
       <c r="H22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -2898,14 +2988,18 @@
       <c r="F23" t="s">
         <v>97</v>
       </c>
-      <c r="G23" t="s">
-        <v>6</v>
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>Pittsburgh, Pennsylvania</v>
       </c>
       <c r="H23" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -2924,14 +3018,18 @@
       <c r="F24" t="s">
         <v>62</v>
       </c>
-      <c r="G24" t="s">
-        <v>6</v>
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>San Diego, California</v>
       </c>
       <c r="H24" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -2950,14 +3048,18 @@
       <c r="F25" t="s">
         <v>62</v>
       </c>
-      <c r="G25" t="s">
-        <v>6</v>
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v>San Francisco, California</v>
       </c>
       <c r="H25" t="s">
+        <v>6</v>
+      </c>
+      <c r="I25" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -2976,14 +3078,18 @@
       <c r="F26" t="s">
         <v>114</v>
       </c>
-      <c r="G26" t="s">
-        <v>6</v>
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v>Seattle, Washington</v>
       </c>
       <c r="H26" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -3002,14 +3108,18 @@
       <c r="F27" t="s">
         <v>57</v>
       </c>
-      <c r="G27" t="s">
-        <v>6</v>
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>St. Louis, Missouri</v>
       </c>
       <c r="H27" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -3029,13 +3139,16 @@
         <v>69</v>
       </c>
       <c r="G28" t="s">
-        <v>6</v>
+        <v>396</v>
       </c>
       <c r="H28" t="s">
+        <v>6</v>
+      </c>
+      <c r="I28" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -3055,13 +3168,16 @@
         <v>52</v>
       </c>
       <c r="G29" t="s">
-        <v>6</v>
+        <v>258</v>
       </c>
       <c r="H29" t="s">
+        <v>6</v>
+      </c>
+      <c r="I29" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -3080,14 +3196,18 @@
       <c r="F30" t="s">
         <v>131</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>Toronto, Ontario</v>
+      </c>
+      <c r="H30" t="s">
         <v>132</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -3106,14 +3226,18 @@
       <c r="F31" t="s">
         <v>136</v>
       </c>
-      <c r="G31" t="s">
-        <v>6</v>
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v>Washington, D.C.</v>
       </c>
       <c r="H31" t="s">
+        <v>6</v>
+      </c>
+      <c r="I31" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>137</v>
       </c>
@@ -3132,14 +3256,18 @@
       <c r="F32" t="s">
         <v>11</v>
       </c>
-      <c r="G32" t="s">
-        <v>6</v>
+      <c r="G32" t="str">
+        <f t="shared" si="0"/>
+        <v>Atlanta, Georgia</v>
       </c>
       <c r="H32" t="s">
+        <v>6</v>
+      </c>
+      <c r="I32" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>137</v>
       </c>
@@ -3158,14 +3286,18 @@
       <c r="F33" t="s">
         <v>52</v>
       </c>
-      <c r="G33" t="s">
-        <v>6</v>
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v>Austin, Texas</v>
       </c>
       <c r="H33" t="s">
+        <v>6</v>
+      </c>
+      <c r="I33" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>137</v>
       </c>
@@ -3184,14 +3316,18 @@
       <c r="F34" t="s">
         <v>149</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v>Montreal, Quebec</v>
+      </c>
+      <c r="H34" t="s">
         <v>132</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>137</v>
       </c>
@@ -3210,14 +3346,18 @@
       <c r="F35" t="s">
         <v>154</v>
       </c>
-      <c r="G35" t="s">
-        <v>6</v>
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v>Charlotte, North Carolina</v>
       </c>
       <c r="H35" t="s">
+        <v>6</v>
+      </c>
+      <c r="I35" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>137</v>
       </c>
@@ -3236,14 +3376,18 @@
       <c r="F36" t="s">
         <v>26</v>
       </c>
-      <c r="G36" t="s">
-        <v>6</v>
+      <c r="G36" t="str">
+        <f t="shared" si="0"/>
+        <v>Chicago, Illinois</v>
       </c>
       <c r="H36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I36" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>137</v>
       </c>
@@ -3263,13 +3407,16 @@
         <v>42</v>
       </c>
       <c r="G37" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="H37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I37" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>137</v>
       </c>
@@ -3288,14 +3435,18 @@
       <c r="F38" t="s">
         <v>33</v>
       </c>
-      <c r="G38" t="s">
-        <v>6</v>
+      <c r="G38" t="str">
+        <f t="shared" si="0"/>
+        <v>Columbus, Ohio</v>
       </c>
       <c r="H38" t="s">
+        <v>6</v>
+      </c>
+      <c r="I38" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>137</v>
       </c>
@@ -3314,14 +3465,18 @@
       <c r="F39" t="s">
         <v>136</v>
       </c>
-      <c r="G39" t="s">
-        <v>6</v>
+      <c r="G39" t="str">
+        <f t="shared" si="0"/>
+        <v>Washington, D.C.</v>
       </c>
       <c r="H39" t="s">
+        <v>6</v>
+      </c>
+      <c r="I39" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>137</v>
       </c>
@@ -3340,14 +3495,18 @@
       <c r="F40" t="s">
         <v>33</v>
       </c>
-      <c r="G40" t="s">
-        <v>6</v>
+      <c r="G40" t="str">
+        <f t="shared" si="0"/>
+        <v>Cincinnati, Ohio</v>
       </c>
       <c r="H40" t="s">
+        <v>6</v>
+      </c>
+      <c r="I40" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>137</v>
       </c>
@@ -3367,13 +3526,16 @@
         <v>52</v>
       </c>
       <c r="G41" t="s">
-        <v>6</v>
+        <v>258</v>
       </c>
       <c r="H41" t="s">
+        <v>6</v>
+      </c>
+      <c r="I41" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>137</v>
       </c>
@@ -3392,14 +3554,18 @@
       <c r="F42" t="s">
         <v>52</v>
       </c>
-      <c r="G42" t="s">
-        <v>6</v>
+      <c r="G42" t="str">
+        <f t="shared" si="0"/>
+        <v>Houston, Texas</v>
       </c>
       <c r="H42" t="s">
+        <v>6</v>
+      </c>
+      <c r="I42" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>137</v>
       </c>
@@ -3419,13 +3585,16 @@
         <v>69</v>
       </c>
       <c r="G43" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="H43" t="s">
+        <v>6</v>
+      </c>
+      <c r="I43" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>137</v>
       </c>
@@ -3444,14 +3613,18 @@
       <c r="F44" t="s">
         <v>62</v>
       </c>
-      <c r="G44" t="s">
-        <v>6</v>
+      <c r="G44" t="str">
+        <f t="shared" si="0"/>
+        <v>Los Angeles, California</v>
       </c>
       <c r="H44" t="s">
+        <v>6</v>
+      </c>
+      <c r="I44" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>137</v>
       </c>
@@ -3471,13 +3644,16 @@
         <v>62</v>
       </c>
       <c r="G45" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="H45" t="s">
+        <v>6</v>
+      </c>
+      <c r="I45" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>137</v>
       </c>
@@ -3497,13 +3673,16 @@
         <v>79</v>
       </c>
       <c r="G46" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="H46" t="s">
+        <v>6</v>
+      </c>
+      <c r="I46" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>137</v>
       </c>
@@ -3522,14 +3701,18 @@
       <c r="F47" t="s">
         <v>193</v>
       </c>
-      <c r="G47" t="s">
-        <v>6</v>
+      <c r="G47" t="str">
+        <f t="shared" si="0"/>
+        <v>Nashville, Tennessee</v>
       </c>
       <c r="H47" t="s">
+        <v>6</v>
+      </c>
+      <c r="I47" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>137</v>
       </c>
@@ -3549,13 +3732,16 @@
         <v>21</v>
       </c>
       <c r="G48" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="H48" t="s">
+        <v>6</v>
+      </c>
+      <c r="I48" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>137</v>
       </c>
@@ -3575,13 +3761,16 @@
         <v>84</v>
       </c>
       <c r="G49" t="s">
-        <v>6</v>
+        <v>293</v>
       </c>
       <c r="H49" t="s">
+        <v>6</v>
+      </c>
+      <c r="I49" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>137</v>
       </c>
@@ -3601,13 +3790,16 @@
         <v>203</v>
       </c>
       <c r="G50" t="s">
-        <v>6</v>
+        <v>293</v>
       </c>
       <c r="H50" t="s">
+        <v>6</v>
+      </c>
+      <c r="I50" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>137</v>
       </c>
@@ -3626,14 +3818,18 @@
       <c r="F51" t="s">
         <v>69</v>
       </c>
-      <c r="G51" t="s">
-        <v>6</v>
+      <c r="G51" t="str">
+        <f t="shared" si="0"/>
+        <v>Orlando, Florida</v>
       </c>
       <c r="H51" t="s">
+        <v>6</v>
+      </c>
+      <c r="I51" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>137</v>
       </c>
@@ -3653,13 +3849,16 @@
         <v>97</v>
       </c>
       <c r="G52" t="s">
-        <v>6</v>
+        <v>95</v>
       </c>
       <c r="H52" t="s">
+        <v>6</v>
+      </c>
+      <c r="I52" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>137</v>
       </c>
@@ -3678,14 +3877,18 @@
       <c r="F53" t="s">
         <v>216</v>
       </c>
-      <c r="G53" t="s">
-        <v>6</v>
+      <c r="G53" t="str">
+        <f t="shared" si="0"/>
+        <v>Portland, Oregon</v>
       </c>
       <c r="H53" t="s">
+        <v>6</v>
+      </c>
+      <c r="I53" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>137</v>
       </c>
@@ -3705,13 +3908,16 @@
         <v>221</v>
       </c>
       <c r="G54" t="s">
-        <v>6</v>
+        <v>320</v>
       </c>
       <c r="H54" t="s">
+        <v>6</v>
+      </c>
+      <c r="I54" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>137</v>
       </c>
@@ -3731,13 +3937,16 @@
         <v>62</v>
       </c>
       <c r="G55" t="s">
-        <v>6</v>
+        <v>108</v>
       </c>
       <c r="H55" t="s">
+        <v>6</v>
+      </c>
+      <c r="I55" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>137</v>
       </c>
@@ -3756,14 +3965,18 @@
       <c r="F56" t="s">
         <v>114</v>
       </c>
-      <c r="G56" t="s">
-        <v>6</v>
+      <c r="G56" t="str">
+        <f t="shared" si="0"/>
+        <v>Seattle, Washington</v>
       </c>
       <c r="H56" t="s">
+        <v>6</v>
+      </c>
+      <c r="I56" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>137</v>
       </c>
@@ -3783,13 +3996,16 @@
         <v>231</v>
       </c>
       <c r="G57" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="H57" t="s">
+        <v>6</v>
+      </c>
+      <c r="I57" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>137</v>
       </c>
@@ -3808,14 +4024,18 @@
       <c r="F58" t="s">
         <v>57</v>
       </c>
-      <c r="G58" t="s">
-        <v>6</v>
+      <c r="G58" t="str">
+        <f t="shared" si="0"/>
+        <v>St. Louis, Missouri</v>
       </c>
       <c r="H58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I58" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>137</v>
       </c>
@@ -3834,14 +4054,18 @@
       <c r="F59" t="s">
         <v>131</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G59" t="str">
+        <f t="shared" si="0"/>
+        <v>Toronto, Ontario</v>
+      </c>
+      <c r="H59" t="s">
         <v>132</v>
       </c>
-      <c r="H59" t="s">
+      <c r="I59" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>137</v>
       </c>
@@ -3860,14 +4084,18 @@
       <c r="F60" t="s">
         <v>240</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G60" t="str">
+        <f t="shared" si="0"/>
+        <v>Vancouver, British Columbia</v>
+      </c>
+      <c r="H60" t="s">
         <v>132</v>
       </c>
-      <c r="H60" t="s">
+      <c r="I60" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>241</v>
       </c>
@@ -3886,14 +4114,18 @@
       <c r="F61" t="s">
         <v>11</v>
       </c>
-      <c r="G61" t="s">
-        <v>6</v>
+      <c r="G61" t="str">
+        <f t="shared" si="0"/>
+        <v>Atlanta, Georgia</v>
       </c>
       <c r="H61" t="s">
+        <v>6</v>
+      </c>
+      <c r="I61" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>241</v>
       </c>
@@ -3912,14 +4144,18 @@
       <c r="F62" t="s">
         <v>21</v>
       </c>
-      <c r="G62" t="s">
-        <v>6</v>
+      <c r="G62" t="str">
+        <f t="shared" si="0"/>
+        <v>Boston, Massachusetts</v>
       </c>
       <c r="H62" t="s">
+        <v>6</v>
+      </c>
+      <c r="I62" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>241</v>
       </c>
@@ -3939,13 +4175,16 @@
         <v>84</v>
       </c>
       <c r="G63" t="s">
-        <v>6</v>
+        <v>293</v>
       </c>
       <c r="H63" t="s">
+        <v>6</v>
+      </c>
+      <c r="I63" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>241</v>
       </c>
@@ -3964,14 +4203,18 @@
       <c r="F64" t="s">
         <v>154</v>
       </c>
-      <c r="G64" t="s">
-        <v>6</v>
+      <c r="G64" t="str">
+        <f t="shared" si="0"/>
+        <v>Charlotte, North Carolina</v>
       </c>
       <c r="H64" t="s">
+        <v>6</v>
+      </c>
+      <c r="I64" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>241</v>
       </c>
@@ -3990,14 +4233,18 @@
       <c r="F65" t="s">
         <v>26</v>
       </c>
-      <c r="G65" t="s">
-        <v>6</v>
+      <c r="G65" t="str">
+        <f t="shared" si="0"/>
+        <v>Chicago, Illinois</v>
       </c>
       <c r="H65" t="s">
+        <v>6</v>
+      </c>
+      <c r="I65" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>241</v>
       </c>
@@ -4016,14 +4263,18 @@
       <c r="F66" t="s">
         <v>33</v>
       </c>
-      <c r="G66" t="s">
-        <v>6</v>
+      <c r="G66" t="str">
+        <f t="shared" si="0"/>
+        <v>Cleveland, Ohio</v>
       </c>
       <c r="H66" t="s">
+        <v>6</v>
+      </c>
+      <c r="I66" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>241</v>
       </c>
@@ -4042,14 +4293,18 @@
       <c r="F67" t="s">
         <v>52</v>
       </c>
-      <c r="G67" t="s">
-        <v>6</v>
+      <c r="G67" t="str">
+        <f t="shared" si="0"/>
+        <v>Dallas, Texas</v>
       </c>
       <c r="H67" t="s">
+        <v>6</v>
+      </c>
+      <c r="I67" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>241</v>
       </c>
@@ -4068,14 +4323,18 @@
       <c r="F68" t="s">
         <v>42</v>
       </c>
-      <c r="G68" t="s">
-        <v>6</v>
+      <c r="G68" t="str">
+        <f t="shared" ref="G68:G131" si="1">D68</f>
+        <v>Denver, Colorado</v>
       </c>
       <c r="H68" t="s">
+        <v>6</v>
+      </c>
+      <c r="I68" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>241</v>
       </c>
@@ -4094,14 +4353,18 @@
       <c r="F69" t="s">
         <v>47</v>
       </c>
-      <c r="G69" t="s">
-        <v>6</v>
+      <c r="G69" t="str">
+        <f t="shared" si="1"/>
+        <v>Detroit, Michigan</v>
       </c>
       <c r="H69" t="s">
+        <v>6</v>
+      </c>
+      <c r="I69" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>241</v>
       </c>
@@ -4120,14 +4383,18 @@
       <c r="F70" t="s">
         <v>62</v>
       </c>
-      <c r="G70" t="s">
-        <v>6</v>
+      <c r="G70" t="str">
+        <f t="shared" si="1"/>
+        <v>San Francisco, California</v>
       </c>
       <c r="H70" t="s">
+        <v>6</v>
+      </c>
+      <c r="I70" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>241</v>
       </c>
@@ -4146,14 +4413,18 @@
       <c r="F71" t="s">
         <v>52</v>
       </c>
-      <c r="G71" t="s">
-        <v>6</v>
+      <c r="G71" t="str">
+        <f t="shared" si="1"/>
+        <v>Houston, Texas</v>
       </c>
       <c r="H71" t="s">
+        <v>6</v>
+      </c>
+      <c r="I71" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>241</v>
       </c>
@@ -4172,14 +4443,18 @@
       <c r="F72" t="s">
         <v>272</v>
       </c>
-      <c r="G72" t="s">
-        <v>6</v>
+      <c r="G72" t="str">
+        <f t="shared" si="1"/>
+        <v>Indianapolis, Indiana</v>
       </c>
       <c r="H72" t="s">
+        <v>6</v>
+      </c>
+      <c r="I72" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>241</v>
       </c>
@@ -4198,14 +4473,18 @@
       <c r="F73" t="s">
         <v>62</v>
       </c>
-      <c r="G73" t="s">
-        <v>6</v>
+      <c r="G73" t="str">
+        <f t="shared" si="1"/>
+        <v>Los Angeles, California</v>
       </c>
       <c r="H73" t="s">
+        <v>6</v>
+      </c>
+      <c r="I73" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>241</v>
       </c>
@@ -4224,14 +4503,18 @@
       <c r="F74" t="s">
         <v>62</v>
       </c>
-      <c r="G74" t="s">
-        <v>6</v>
+      <c r="G74" t="str">
+        <f t="shared" si="1"/>
+        <v>Los Angeles, California</v>
       </c>
       <c r="H74" t="s">
+        <v>6</v>
+      </c>
+      <c r="I74" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>241</v>
       </c>
@@ -4250,14 +4533,18 @@
       <c r="F75" t="s">
         <v>193</v>
       </c>
-      <c r="G75" t="s">
-        <v>6</v>
+      <c r="G75" t="str">
+        <f t="shared" si="1"/>
+        <v>Memphis, Tennessee</v>
       </c>
       <c r="H75" t="s">
+        <v>6</v>
+      </c>
+      <c r="I75" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>241</v>
       </c>
@@ -4276,14 +4563,18 @@
       <c r="F76" t="s">
         <v>69</v>
       </c>
-      <c r="G76" t="s">
-        <v>6</v>
+      <c r="G76" t="str">
+        <f t="shared" si="1"/>
+        <v>Miami, Florida</v>
       </c>
       <c r="H76" t="s">
+        <v>6</v>
+      </c>
+      <c r="I76" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>241</v>
       </c>
@@ -4302,14 +4593,18 @@
       <c r="F77" t="s">
         <v>74</v>
       </c>
-      <c r="G77" t="s">
-        <v>6</v>
+      <c r="G77" t="str">
+        <f t="shared" si="1"/>
+        <v>Milwaukee, Wisconsin</v>
       </c>
       <c r="H77" t="s">
+        <v>6</v>
+      </c>
+      <c r="I77" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>241</v>
       </c>
@@ -4328,14 +4623,18 @@
       <c r="F78" t="s">
         <v>79</v>
       </c>
-      <c r="G78" t="s">
-        <v>6</v>
+      <c r="G78" t="str">
+        <f t="shared" si="1"/>
+        <v>Minneapolis, Minnesota</v>
       </c>
       <c r="H78" t="s">
+        <v>6</v>
+      </c>
+      <c r="I78" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>241</v>
       </c>
@@ -4354,14 +4653,18 @@
       <c r="F79" t="s">
         <v>290</v>
       </c>
-      <c r="G79" t="s">
-        <v>6</v>
+      <c r="G79" t="str">
+        <f t="shared" si="1"/>
+        <v>New Orleans, Louisiana</v>
       </c>
       <c r="H79" t="s">
+        <v>6</v>
+      </c>
+      <c r="I79" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>241</v>
       </c>
@@ -4380,14 +4683,18 @@
       <c r="F80" t="s">
         <v>84</v>
       </c>
-      <c r="G80" t="s">
-        <v>6</v>
+      <c r="G80" t="str">
+        <f t="shared" si="1"/>
+        <v>New York City, New York</v>
       </c>
       <c r="H80" t="s">
+        <v>6</v>
+      </c>
+      <c r="I80" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>241</v>
       </c>
@@ -4406,14 +4713,18 @@
       <c r="F81" t="s">
         <v>299</v>
       </c>
-      <c r="G81" t="s">
-        <v>6</v>
+      <c r="G81" t="str">
+        <f t="shared" si="1"/>
+        <v>Oklahoma City, Oklahoma</v>
       </c>
       <c r="H81" t="s">
+        <v>6</v>
+      </c>
+      <c r="I81" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>241</v>
       </c>
@@ -4432,14 +4743,18 @@
       <c r="F82" t="s">
         <v>69</v>
       </c>
-      <c r="G82" t="s">
-        <v>6</v>
+      <c r="G82" t="str">
+        <f t="shared" si="1"/>
+        <v>Orlando, Florida</v>
       </c>
       <c r="H82" t="s">
+        <v>6</v>
+      </c>
+      <c r="I82" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>241</v>
       </c>
@@ -4458,14 +4773,18 @@
       <c r="F83" t="s">
         <v>97</v>
       </c>
-      <c r="G83" t="s">
-        <v>6</v>
+      <c r="G83" t="str">
+        <f t="shared" si="1"/>
+        <v>Philadelphia, Pennsylvania</v>
       </c>
       <c r="H83" t="s">
+        <v>6</v>
+      </c>
+      <c r="I83" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>241</v>
       </c>
@@ -4484,14 +4803,18 @@
       <c r="F84" t="s">
         <v>5</v>
       </c>
-      <c r="G84" t="s">
-        <v>6</v>
+      <c r="G84" t="str">
+        <f t="shared" si="1"/>
+        <v>Phoenix, Arizona</v>
       </c>
       <c r="H84" t="s">
+        <v>6</v>
+      </c>
+      <c r="I84" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>241</v>
       </c>
@@ -4510,14 +4833,18 @@
       <c r="F85" t="s">
         <v>216</v>
       </c>
-      <c r="G85" t="s">
-        <v>6</v>
+      <c r="G85" t="str">
+        <f t="shared" si="1"/>
+        <v>Portland, Oregon</v>
       </c>
       <c r="H85" t="s">
+        <v>6</v>
+      </c>
+      <c r="I85" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>241</v>
       </c>
@@ -4536,14 +4863,18 @@
       <c r="F86" t="s">
         <v>62</v>
       </c>
-      <c r="G86" t="s">
-        <v>6</v>
+      <c r="G86" t="str">
+        <f t="shared" si="1"/>
+        <v>Sacramento, California</v>
       </c>
       <c r="H86" t="s">
+        <v>6</v>
+      </c>
+      <c r="I86" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>241</v>
       </c>
@@ -4562,14 +4893,18 @@
       <c r="F87" t="s">
         <v>52</v>
       </c>
-      <c r="G87" t="s">
-        <v>6</v>
+      <c r="G87" t="str">
+        <f t="shared" si="1"/>
+        <v>San Antonio, Texas</v>
       </c>
       <c r="H87" t="s">
+        <v>6</v>
+      </c>
+      <c r="I87" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>241</v>
       </c>
@@ -4588,14 +4923,18 @@
       <c r="F88" t="s">
         <v>131</v>
       </c>
-      <c r="G88" t="s">
+      <c r="G88" t="str">
+        <f t="shared" si="1"/>
+        <v>Toronto, Ontario</v>
+      </c>
+      <c r="H88" t="s">
         <v>132</v>
       </c>
-      <c r="H88" t="s">
+      <c r="I88" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>241</v>
       </c>
@@ -4614,14 +4953,18 @@
       <c r="F89" t="s">
         <v>221</v>
       </c>
-      <c r="G89" t="s">
-        <v>6</v>
+      <c r="G89" t="str">
+        <f t="shared" si="1"/>
+        <v>Salt Lake City, Utah</v>
       </c>
       <c r="H89" t="s">
+        <v>6</v>
+      </c>
+      <c r="I89" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>241</v>
       </c>
@@ -4640,14 +4983,18 @@
       <c r="F90" t="s">
         <v>136</v>
       </c>
-      <c r="G90" t="s">
-        <v>6</v>
+      <c r="G90" t="str">
+        <f t="shared" si="1"/>
+        <v>Washington, D.C.</v>
       </c>
       <c r="H90" t="s">
+        <v>6</v>
+      </c>
+      <c r="I90" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>324</v>
       </c>
@@ -4667,13 +5014,16 @@
         <v>5</v>
       </c>
       <c r="G91" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H91" t="s">
+        <v>6</v>
+      </c>
+      <c r="I91" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>324</v>
       </c>
@@ -4692,14 +5042,18 @@
       <c r="F92" t="s">
         <v>11</v>
       </c>
-      <c r="G92" t="s">
-        <v>6</v>
+      <c r="G92" t="str">
+        <f t="shared" si="1"/>
+        <v>Atlanta, Georgia</v>
       </c>
       <c r="H92" t="s">
+        <v>6</v>
+      </c>
+      <c r="I92" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>324</v>
       </c>
@@ -4718,14 +5072,18 @@
       <c r="F93" t="s">
         <v>16</v>
       </c>
-      <c r="G93" t="s">
-        <v>6</v>
+      <c r="G93" t="str">
+        <f t="shared" si="1"/>
+        <v>Baltimore, Maryland</v>
       </c>
       <c r="H93" t="s">
+        <v>6</v>
+      </c>
+      <c r="I93" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>324</v>
       </c>
@@ -4745,13 +5103,16 @@
         <v>84</v>
       </c>
       <c r="G94" t="s">
-        <v>6</v>
+        <v>412</v>
       </c>
       <c r="H94" t="s">
+        <v>6</v>
+      </c>
+      <c r="I94" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>324</v>
       </c>
@@ -4770,14 +5131,18 @@
       <c r="F95" t="s">
         <v>154</v>
       </c>
-      <c r="G95" t="s">
-        <v>6</v>
+      <c r="G95" t="str">
+        <f t="shared" si="1"/>
+        <v>Charlotte, North Carolina</v>
       </c>
       <c r="H95" t="s">
+        <v>6</v>
+      </c>
+      <c r="I95" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>324</v>
       </c>
@@ -4796,14 +5161,18 @@
       <c r="F96" t="s">
         <v>26</v>
       </c>
-      <c r="G96" t="s">
-        <v>6</v>
+      <c r="G96" t="str">
+        <f t="shared" si="1"/>
+        <v>Chicago, Illinois</v>
       </c>
       <c r="H96" t="s">
+        <v>6</v>
+      </c>
+      <c r="I96" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>324</v>
       </c>
@@ -4822,14 +5191,18 @@
       <c r="F97" t="s">
         <v>33</v>
       </c>
-      <c r="G97" t="s">
-        <v>6</v>
+      <c r="G97" t="str">
+        <f t="shared" si="1"/>
+        <v>Cincinnati, Ohio</v>
       </c>
       <c r="H97" t="s">
+        <v>6</v>
+      </c>
+      <c r="I97" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>324</v>
       </c>
@@ -4848,14 +5221,18 @@
       <c r="F98" t="s">
         <v>33</v>
       </c>
-      <c r="G98" t="s">
-        <v>6</v>
+      <c r="G98" t="str">
+        <f t="shared" si="1"/>
+        <v>Cleveland, Ohio</v>
       </c>
       <c r="H98" t="s">
+        <v>6</v>
+      </c>
+      <c r="I98" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>324</v>
       </c>
@@ -4875,13 +5252,16 @@
         <v>52</v>
       </c>
       <c r="G99" t="s">
-        <v>6</v>
+        <v>258</v>
       </c>
       <c r="H99" t="s">
+        <v>6</v>
+      </c>
+      <c r="I99" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>324</v>
       </c>
@@ -4900,14 +5280,18 @@
       <c r="F100" t="s">
         <v>42</v>
       </c>
-      <c r="G100" t="s">
-        <v>6</v>
+      <c r="G100" t="str">
+        <f t="shared" si="1"/>
+        <v>Denver, Colorado</v>
       </c>
       <c r="H100" t="s">
+        <v>6</v>
+      </c>
+      <c r="I100" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>324</v>
       </c>
@@ -4926,14 +5310,18 @@
       <c r="F101" t="s">
         <v>47</v>
       </c>
-      <c r="G101" t="s">
-        <v>6</v>
+      <c r="G101" t="str">
+        <f t="shared" si="1"/>
+        <v>Detroit, Michigan</v>
       </c>
       <c r="H101" t="s">
+        <v>6</v>
+      </c>
+      <c r="I101" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>324</v>
       </c>
@@ -4952,14 +5340,18 @@
       <c r="F102" t="s">
         <v>74</v>
       </c>
-      <c r="G102" t="s">
-        <v>6</v>
+      <c r="G102" t="str">
+        <f t="shared" si="1"/>
+        <v>Green Bay, Wisconsin</v>
       </c>
       <c r="H102" t="s">
+        <v>6</v>
+      </c>
+      <c r="I102" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>324</v>
       </c>
@@ -4978,14 +5370,18 @@
       <c r="F103" t="s">
         <v>52</v>
       </c>
-      <c r="G103" t="s">
-        <v>6</v>
+      <c r="G103" t="str">
+        <f t="shared" si="1"/>
+        <v>Houston, Texas</v>
       </c>
       <c r="H103" t="s">
+        <v>6</v>
+      </c>
+      <c r="I103" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>324</v>
       </c>
@@ -5004,14 +5400,18 @@
       <c r="F104" t="s">
         <v>272</v>
       </c>
-      <c r="G104" t="s">
-        <v>6</v>
+      <c r="G104" t="str">
+        <f t="shared" si="1"/>
+        <v>Indianapolis, Indiana</v>
       </c>
       <c r="H104" t="s">
+        <v>6</v>
+      </c>
+      <c r="I104" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>324</v>
       </c>
@@ -5030,14 +5430,18 @@
       <c r="F105" t="s">
         <v>69</v>
       </c>
-      <c r="G105" t="s">
-        <v>6</v>
+      <c r="G105" t="str">
+        <f t="shared" si="1"/>
+        <v>Jacksonville, Florida</v>
       </c>
       <c r="H105" t="s">
+        <v>6</v>
+      </c>
+      <c r="I105" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>324</v>
       </c>
@@ -5056,14 +5460,18 @@
       <c r="F106" t="s">
         <v>57</v>
       </c>
-      <c r="G106" t="s">
-        <v>6</v>
+      <c r="G106" t="str">
+        <f t="shared" si="1"/>
+        <v>Kansas City, Missouri</v>
       </c>
       <c r="H106" t="s">
+        <v>6</v>
+      </c>
+      <c r="I106" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>324</v>
       </c>
@@ -5083,13 +5491,16 @@
         <v>365</v>
       </c>
       <c r="G107" t="s">
-        <v>6</v>
+        <v>626</v>
       </c>
       <c r="H107" t="s">
+        <v>6</v>
+      </c>
+      <c r="I107" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>324</v>
       </c>
@@ -5109,13 +5520,16 @@
         <v>62</v>
       </c>
       <c r="G108" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="H108" t="s">
+        <v>6</v>
+      </c>
+      <c r="I108" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>324</v>
       </c>
@@ -5135,13 +5549,16 @@
         <v>62</v>
       </c>
       <c r="G109" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="H109" t="s">
+        <v>6</v>
+      </c>
+      <c r="I109" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>324</v>
       </c>
@@ -5161,13 +5578,16 @@
         <v>69</v>
       </c>
       <c r="G110" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="H110" t="s">
+        <v>6</v>
+      </c>
+      <c r="I110" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>324</v>
       </c>
@@ -5186,14 +5606,18 @@
       <c r="F111" t="s">
         <v>79</v>
       </c>
-      <c r="G111" t="s">
-        <v>6</v>
+      <c r="G111" t="str">
+        <f t="shared" si="1"/>
+        <v>Minneapolis, Minnesota</v>
       </c>
       <c r="H111" t="s">
+        <v>6</v>
+      </c>
+      <c r="I111" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>324</v>
       </c>
@@ -5213,13 +5637,16 @@
         <v>21</v>
       </c>
       <c r="G112" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="H112" t="s">
+        <v>6</v>
+      </c>
+      <c r="I112" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>324</v>
       </c>
@@ -5238,14 +5665,18 @@
       <c r="F113" t="s">
         <v>290</v>
       </c>
-      <c r="G113" t="s">
-        <v>6</v>
+      <c r="G113" t="str">
+        <f t="shared" si="1"/>
+        <v>New Orleans, Louisiana</v>
       </c>
       <c r="H113" t="s">
+        <v>6</v>
+      </c>
+      <c r="I113" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>324</v>
       </c>
@@ -5265,13 +5696,16 @@
         <v>203</v>
       </c>
       <c r="G114" t="s">
-        <v>6</v>
+        <v>293</v>
       </c>
       <c r="H114" t="s">
+        <v>6</v>
+      </c>
+      <c r="I114" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>324</v>
       </c>
@@ -5291,13 +5725,16 @@
         <v>203</v>
       </c>
       <c r="G115" t="s">
-        <v>6</v>
+        <v>293</v>
       </c>
       <c r="H115" t="s">
+        <v>6</v>
+      </c>
+      <c r="I115" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>324</v>
       </c>
@@ -5316,14 +5753,18 @@
       <c r="F116" t="s">
         <v>97</v>
       </c>
-      <c r="G116" t="s">
-        <v>6</v>
+      <c r="G116" t="str">
+        <f t="shared" si="1"/>
+        <v>Philadelphia, Pennsylvania</v>
       </c>
       <c r="H116" t="s">
+        <v>6</v>
+      </c>
+      <c r="I116" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>324</v>
       </c>
@@ -5342,14 +5783,18 @@
       <c r="F117" t="s">
         <v>97</v>
       </c>
-      <c r="G117" t="s">
-        <v>6</v>
+      <c r="G117" t="str">
+        <f t="shared" si="1"/>
+        <v>Pittsburgh, Pennsylvania</v>
       </c>
       <c r="H117" t="s">
+        <v>6</v>
+      </c>
+      <c r="I117" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>324</v>
       </c>
@@ -5369,13 +5814,16 @@
         <v>62</v>
       </c>
       <c r="G118" t="s">
-        <v>6</v>
+        <v>108</v>
       </c>
       <c r="H118" t="s">
+        <v>6</v>
+      </c>
+      <c r="I118" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>324</v>
       </c>
@@ -5394,14 +5842,18 @@
       <c r="F119" t="s">
         <v>114</v>
       </c>
-      <c r="G119" t="s">
-        <v>6</v>
+      <c r="G119" t="str">
+        <f t="shared" si="1"/>
+        <v>Seattle, Washington</v>
       </c>
       <c r="H119" t="s">
+        <v>6</v>
+      </c>
+      <c r="I119" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>324</v>
       </c>
@@ -5420,14 +5872,18 @@
       <c r="F120" t="s">
         <v>69</v>
       </c>
-      <c r="G120" t="s">
-        <v>6</v>
+      <c r="G120" t="str">
+        <f t="shared" si="1"/>
+        <v>Tampa, Florida</v>
       </c>
       <c r="H120" t="s">
+        <v>6</v>
+      </c>
+      <c r="I120" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>324</v>
       </c>
@@ -5446,14 +5902,18 @@
       <c r="F121" t="s">
         <v>193</v>
       </c>
-      <c r="G121" t="s">
-        <v>6</v>
+      <c r="G121" t="str">
+        <f t="shared" si="1"/>
+        <v>Nashville, Tennessee</v>
       </c>
       <c r="H121" t="s">
+        <v>6</v>
+      </c>
+      <c r="I121" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>324</v>
       </c>
@@ -5473,13 +5933,16 @@
         <v>16</v>
       </c>
       <c r="G122" t="s">
-        <v>6</v>
+        <v>135</v>
       </c>
       <c r="H122" t="s">
+        <v>6</v>
+      </c>
+      <c r="I122" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>404</v>
       </c>
@@ -5499,13 +5962,16 @@
         <v>62</v>
       </c>
       <c r="G123" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="H123" t="s">
+        <v>6</v>
+      </c>
+      <c r="I123" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>404</v>
       </c>
@@ -5524,14 +5990,18 @@
       <c r="F124" t="s">
         <v>221</v>
       </c>
-      <c r="G124" t="s">
-        <v>6</v>
+      <c r="G124" t="str">
+        <f t="shared" si="1"/>
+        <v>Salt Lake City, Utah</v>
       </c>
       <c r="H124" t="s">
+        <v>6</v>
+      </c>
+      <c r="I124" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>404</v>
       </c>
@@ -5550,14 +6020,18 @@
       <c r="F125" t="s">
         <v>21</v>
       </c>
-      <c r="G125" t="s">
-        <v>6</v>
+      <c r="G125" t="str">
+        <f t="shared" si="1"/>
+        <v>Boston, Massachusetts</v>
       </c>
       <c r="H125" t="s">
+        <v>6</v>
+      </c>
+      <c r="I125" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>404</v>
       </c>
@@ -5576,14 +6050,18 @@
       <c r="F126" t="s">
         <v>84</v>
       </c>
-      <c r="G126" t="s">
-        <v>6</v>
+      <c r="G126" t="str">
+        <f t="shared" si="1"/>
+        <v>Buffalo, New York</v>
       </c>
       <c r="H126" t="s">
+        <v>6</v>
+      </c>
+      <c r="I126" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>404</v>
       </c>
@@ -5602,14 +6080,18 @@
       <c r="F127" t="s">
         <v>418</v>
       </c>
-      <c r="G127" t="s">
+      <c r="G127" t="str">
+        <f t="shared" si="1"/>
+        <v>Calgary, Alberta</v>
+      </c>
+      <c r="H127" t="s">
         <v>132</v>
       </c>
-      <c r="H127" t="s">
+      <c r="I127" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>404</v>
       </c>
@@ -5628,14 +6110,18 @@
       <c r="F128" t="s">
         <v>154</v>
       </c>
-      <c r="G128" t="s">
-        <v>6</v>
+      <c r="G128" t="str">
+        <f t="shared" si="1"/>
+        <v>Raleigh, North Carolina</v>
       </c>
       <c r="H128" t="s">
+        <v>6</v>
+      </c>
+      <c r="I128" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>404</v>
       </c>
@@ -5654,14 +6140,18 @@
       <c r="F129" t="s">
         <v>26</v>
       </c>
-      <c r="G129" t="s">
-        <v>6</v>
+      <c r="G129" t="str">
+        <f t="shared" si="1"/>
+        <v>Chicago, Illinois</v>
       </c>
       <c r="H129" t="s">
+        <v>6</v>
+      </c>
+      <c r="I129" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>404</v>
       </c>
@@ -5680,14 +6170,18 @@
       <c r="F130" t="s">
         <v>42</v>
       </c>
-      <c r="G130" t="s">
-        <v>6</v>
+      <c r="G130" t="str">
+        <f t="shared" si="1"/>
+        <v>Denver, Colorado</v>
       </c>
       <c r="H130" t="s">
+        <v>6</v>
+      </c>
+      <c r="I130" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>404</v>
       </c>
@@ -5706,14 +6200,18 @@
       <c r="F131" t="s">
         <v>33</v>
       </c>
-      <c r="G131" t="s">
-        <v>6</v>
+      <c r="G131" t="str">
+        <f t="shared" si="1"/>
+        <v>Columbus, Ohio</v>
       </c>
       <c r="H131" t="s">
+        <v>6</v>
+      </c>
+      <c r="I131" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>404</v>
       </c>
@@ -5732,14 +6230,18 @@
       <c r="F132" t="s">
         <v>52</v>
       </c>
-      <c r="G132" t="s">
-        <v>6</v>
+      <c r="G132" t="str">
+        <f t="shared" ref="G132:G155" si="2">D132</f>
+        <v>Dallas, Texas</v>
       </c>
       <c r="H132" t="s">
+        <v>6</v>
+      </c>
+      <c r="I132" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>404</v>
       </c>
@@ -5758,14 +6260,18 @@
       <c r="F133" t="s">
         <v>47</v>
       </c>
-      <c r="G133" t="s">
-        <v>6</v>
+      <c r="G133" t="str">
+        <f t="shared" si="2"/>
+        <v>Detroit, Michigan</v>
       </c>
       <c r="H133" t="s">
+        <v>6</v>
+      </c>
+      <c r="I133" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>404</v>
       </c>
@@ -5784,14 +6290,18 @@
       <c r="F134" t="s">
         <v>418</v>
       </c>
-      <c r="G134" t="s">
+      <c r="G134" t="str">
+        <f t="shared" si="2"/>
+        <v>Edmonton, Alberta</v>
+      </c>
+      <c r="H134" t="s">
         <v>132</v>
       </c>
-      <c r="H134" t="s">
+      <c r="I134" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>404</v>
       </c>
@@ -5811,13 +6321,16 @@
         <v>69</v>
       </c>
       <c r="G135" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="H135" t="s">
+        <v>6</v>
+      </c>
+      <c r="I135" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>404</v>
       </c>
@@ -5836,14 +6349,18 @@
       <c r="F136" t="s">
         <v>62</v>
       </c>
-      <c r="G136" t="s">
-        <v>6</v>
+      <c r="G136" t="str">
+        <f t="shared" si="2"/>
+        <v>Los Angeles, California</v>
       </c>
       <c r="H136" t="s">
+        <v>6</v>
+      </c>
+      <c r="I136" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>404</v>
       </c>
@@ -5863,13 +6380,16 @@
         <v>79</v>
       </c>
       <c r="G137" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="H137" t="s">
+        <v>6</v>
+      </c>
+      <c r="I137" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>404</v>
       </c>
@@ -5888,14 +6408,18 @@
       <c r="F138" t="s">
         <v>149</v>
       </c>
-      <c r="G138" t="s">
+      <c r="G138" t="str">
+        <f t="shared" si="2"/>
+        <v>Montreal, Quebec</v>
+      </c>
+      <c r="H138" t="s">
         <v>132</v>
       </c>
-      <c r="H138" t="s">
+      <c r="I138" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>404</v>
       </c>
@@ -5914,14 +6438,18 @@
       <c r="F139" t="s">
         <v>193</v>
       </c>
-      <c r="G139" t="s">
-        <v>6</v>
+      <c r="G139" t="str">
+        <f t="shared" si="2"/>
+        <v>Nashville, Tennessee</v>
       </c>
       <c r="H139" t="s">
+        <v>6</v>
+      </c>
+      <c r="I139" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>404</v>
       </c>
@@ -5941,13 +6469,16 @@
         <v>203</v>
       </c>
       <c r="G140" t="s">
-        <v>6</v>
+        <v>293</v>
       </c>
       <c r="H140" t="s">
+        <v>6</v>
+      </c>
+      <c r="I140" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>404</v>
       </c>
@@ -5967,13 +6498,16 @@
         <v>84</v>
       </c>
       <c r="G141" t="s">
-        <v>6</v>
+        <v>293</v>
       </c>
       <c r="H141" t="s">
+        <v>6</v>
+      </c>
+      <c r="I141" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>404</v>
       </c>
@@ -5993,13 +6527,16 @@
         <v>84</v>
       </c>
       <c r="G142" t="s">
-        <v>6</v>
+        <v>293</v>
       </c>
       <c r="H142" t="s">
+        <v>6</v>
+      </c>
+      <c r="I142" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>404</v>
       </c>
@@ -6018,14 +6555,18 @@
       <c r="F143" t="s">
         <v>84</v>
       </c>
-      <c r="G143" t="s">
-        <v>6</v>
+      <c r="G143" t="str">
+        <f t="shared" si="2"/>
+        <v>New York City, New York</v>
       </c>
       <c r="H143" t="s">
+        <v>6</v>
+      </c>
+      <c r="I143" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>404</v>
       </c>
@@ -6044,14 +6585,18 @@
       <c r="F144" t="s">
         <v>131</v>
       </c>
-      <c r="G144" t="s">
+      <c r="G144" t="str">
+        <f t="shared" si="2"/>
+        <v>Ottawa, Ontario</v>
+      </c>
+      <c r="H144" t="s">
         <v>132</v>
       </c>
-      <c r="H144" t="s">
+      <c r="I144" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>404</v>
       </c>
@@ -6070,14 +6615,18 @@
       <c r="F145" t="s">
         <v>97</v>
       </c>
-      <c r="G145" t="s">
-        <v>6</v>
+      <c r="G145" t="str">
+        <f t="shared" si="2"/>
+        <v>Philadelphia, Pennsylvania</v>
       </c>
       <c r="H145" t="s">
+        <v>6</v>
+      </c>
+      <c r="I145" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>404</v>
       </c>
@@ -6096,14 +6645,18 @@
       <c r="F146" t="s">
         <v>97</v>
       </c>
-      <c r="G146" t="s">
-        <v>6</v>
+      <c r="G146" t="str">
+        <f t="shared" si="2"/>
+        <v>Pittsburgh, Pennsylvania</v>
       </c>
       <c r="H146" t="s">
+        <v>6</v>
+      </c>
+      <c r="I146" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>404</v>
       </c>
@@ -6123,13 +6676,16 @@
         <v>62</v>
       </c>
       <c r="G147" t="s">
-        <v>6</v>
+        <v>108</v>
       </c>
       <c r="H147" t="s">
+        <v>6</v>
+      </c>
+      <c r="I147" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>404</v>
       </c>
@@ -6148,14 +6704,18 @@
       <c r="F148" t="s">
         <v>114</v>
       </c>
-      <c r="G148" t="s">
-        <v>6</v>
+      <c r="G148" t="str">
+        <f t="shared" si="2"/>
+        <v>Seattle, Washington</v>
       </c>
       <c r="H148" t="s">
+        <v>6</v>
+      </c>
+      <c r="I148" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>404</v>
       </c>
@@ -6174,14 +6734,18 @@
       <c r="F149" t="s">
         <v>57</v>
       </c>
-      <c r="G149" t="s">
-        <v>6</v>
+      <c r="G149" t="str">
+        <f t="shared" si="2"/>
+        <v>St. Louis, Missouri</v>
       </c>
       <c r="H149" t="s">
+        <v>6</v>
+      </c>
+      <c r="I149" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>404</v>
       </c>
@@ -6200,14 +6764,18 @@
       <c r="F150" t="s">
         <v>69</v>
       </c>
-      <c r="G150" t="s">
-        <v>6</v>
+      <c r="G150" t="str">
+        <f t="shared" si="2"/>
+        <v>Tampa, Florida</v>
       </c>
       <c r="H150" t="s">
+        <v>6</v>
+      </c>
+      <c r="I150" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>404</v>
       </c>
@@ -6226,14 +6794,18 @@
       <c r="F151" t="s">
         <v>131</v>
       </c>
-      <c r="G151" t="s">
+      <c r="G151" t="str">
+        <f t="shared" si="2"/>
+        <v>Toronto, Ontario</v>
+      </c>
+      <c r="H151" t="s">
         <v>132</v>
       </c>
-      <c r="H151" t="s">
+      <c r="I151" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>404</v>
       </c>
@@ -6252,14 +6824,18 @@
       <c r="F152" t="s">
         <v>240</v>
       </c>
-      <c r="G152" t="s">
+      <c r="G152" t="str">
+        <f t="shared" si="2"/>
+        <v>Vancouver, British Columbia</v>
+      </c>
+      <c r="H152" t="s">
         <v>132</v>
       </c>
-      <c r="H152" t="s">
+      <c r="I152" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>404</v>
       </c>
@@ -6279,13 +6855,16 @@
         <v>365</v>
       </c>
       <c r="G153" t="s">
-        <v>6</v>
+        <v>626</v>
       </c>
       <c r="H153" t="s">
+        <v>6</v>
+      </c>
+      <c r="I153" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>404</v>
       </c>
@@ -6304,14 +6883,18 @@
       <c r="F154" t="s">
         <v>136</v>
       </c>
-      <c r="G154" t="s">
-        <v>6</v>
+      <c r="G154" t="str">
+        <f t="shared" si="2"/>
+        <v>Washington, D.C.</v>
       </c>
       <c r="H154" t="s">
+        <v>6</v>
+      </c>
+      <c r="I154" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>404</v>
       </c>
@@ -6330,15 +6913,19 @@
       <c r="F155" t="s">
         <v>475</v>
       </c>
-      <c r="G155" t="s">
+      <c r="G155" t="str">
+        <f t="shared" si="2"/>
+        <v>Winnipeg, Manitoba</v>
+      </c>
+      <c r="H155" t="s">
         <v>132</v>
       </c>
-      <c r="H155" t="s">
+      <c r="I155" t="s">
         <v>588</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H156">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I156">
     <sortCondition ref="A2:A156"/>
     <sortCondition ref="B2:B156"/>
   </sortState>

</xml_diff>